<commit_message>
tz: add some form
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Tanzania/tz_sch_sth_impact_202311_1_school.xlsx
+++ b/SCH-STH/Impact assessments/Tanzania/tz_sch_sth_impact_202311_1_school.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Tanzania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A3D1D2-1A9C-4119-B1F9-6A64433FE405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD509017-6CA2-4C12-9C18-CDB1FEB96199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3669" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3669" uniqueCount="634">
   <si>
     <t>type</t>
   </si>
@@ -1550,9 +1550,6 @@
     <t>Hawajawahi</t>
   </si>
   <si>
-    <t>Don't know</t>
-  </si>
-  <si>
     <t>1 month</t>
   </si>
   <si>
@@ -1682,9 +1679,6 @@
     <t>Vyanzo vingine (taja)</t>
   </si>
   <si>
-    <t>Don't know/unsure</t>
-  </si>
-  <si>
     <t>Sijui/hauna uhakika</t>
   </si>
   <si>
@@ -1779,9 +1773,6 @@
   </si>
   <si>
     <t>Siwezi kukifikia choo (chagua jibu hili wakati ambao huwezi kwenda kuona choo tu)</t>
-  </si>
-  <si>
-    <t>Don't.know/unsure</t>
   </si>
   <si>
     <t>Other.(Specify)</t>
@@ -2001,6 +1992,12 @@
   </si>
   <si>
     <t>Ask if the answer is something else</t>
+  </si>
+  <si>
+    <t>Don.t.know/unsure</t>
+  </si>
+  <si>
+    <t>Do not know/unsure</t>
   </si>
 </sst>
 </file>
@@ -2692,8 +2689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
@@ -2976,17 +2973,17 @@
     </row>
     <row r="9" spans="1:15" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="35" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="F9" s="35"/>
       <c r="G9" s="25"/>
@@ -3006,14 +3003,14 @@
         <v>24</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="35" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="F10" s="35"/>
       <c r="G10" s="25"/>
@@ -3033,25 +3030,25 @@
         <v>24</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="35" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="F11" s="35"/>
       <c r="G11" s="25"/>
       <c r="H11" s="25" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="J11" s="35" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="K11" s="25"/>
       <c r="L11" s="25"/>
@@ -3072,7 +3069,7 @@
         <v>412</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>413</v>
@@ -3103,7 +3100,7 @@
         <v>415</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>416</v>
@@ -3134,7 +3131,7 @@
         <v>417</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>418</v>
@@ -3175,7 +3172,7 @@
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="25" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="I15" s="27" t="s">
         <v>423</v>
@@ -3212,7 +3209,7 @@
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="I16" s="27" t="s">
         <v>427</v>
@@ -3249,7 +3246,7 @@
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="I17" s="27" t="s">
         <v>431</v>
@@ -3609,7 +3606,7 @@
         <v>486</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="E29" s="35" t="s">
         <v>487</v>
@@ -3791,9 +3788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H563"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4011,10 +4008,10 @@
         <v>502</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>504</v>
+        <v>336</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>504</v>
+        <v>336</v>
       </c>
       <c r="D13" s="46" t="s">
         <v>492</v>
@@ -4029,13 +4026,13 @@
         <v>502</v>
       </c>
       <c r="B14" s="44" t="s">
+        <v>504</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>504</v>
+      </c>
+      <c r="D14" s="46" t="s">
         <v>505</v>
-      </c>
-      <c r="C14" s="45" t="s">
-        <v>505</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>506</v>
       </c>
       <c r="E14" s="45"/>
       <c r="F14" s="47"/>
@@ -4047,13 +4044,13 @@
         <v>502</v>
       </c>
       <c r="B15" s="44" t="s">
+        <v>506</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>506</v>
+      </c>
+      <c r="D15" s="46" t="s">
         <v>507</v>
-      </c>
-      <c r="C15" s="45" t="s">
-        <v>507</v>
-      </c>
-      <c r="D15" s="46" t="s">
-        <v>508</v>
       </c>
       <c r="E15" s="45"/>
       <c r="F15" s="47"/>
@@ -4065,13 +4062,13 @@
         <v>502</v>
       </c>
       <c r="B16" s="44" t="s">
+        <v>508</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>508</v>
+      </c>
+      <c r="D16" s="46" t="s">
         <v>509</v>
-      </c>
-      <c r="C16" s="45" t="s">
-        <v>509</v>
-      </c>
-      <c r="D16" s="46" t="s">
-        <v>510</v>
       </c>
       <c r="E16" s="45"/>
       <c r="F16" s="47"/>
@@ -4083,13 +4080,13 @@
         <v>502</v>
       </c>
       <c r="B17" s="44" t="s">
+        <v>510</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>510</v>
+      </c>
+      <c r="D17" s="46" t="s">
         <v>511</v>
-      </c>
-      <c r="C17" s="45" t="s">
-        <v>511</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>512</v>
       </c>
       <c r="E17" s="45"/>
       <c r="F17" s="47"/>
@@ -4101,13 +4098,13 @@
         <v>502</v>
       </c>
       <c r="B18" s="44" t="s">
+        <v>512</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>512</v>
+      </c>
+      <c r="D18" s="46" t="s">
         <v>513</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>513</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>514</v>
       </c>
       <c r="E18" s="45"/>
       <c r="F18" s="47"/>
@@ -4119,13 +4116,13 @@
         <v>502</v>
       </c>
       <c r="B19" s="44" t="s">
+        <v>514</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>514</v>
+      </c>
+      <c r="D19" s="46" t="s">
         <v>515</v>
-      </c>
-      <c r="C19" s="45" t="s">
-        <v>515</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>516</v>
       </c>
       <c r="E19" s="45"/>
       <c r="F19" s="47"/>
@@ -4137,13 +4134,13 @@
         <v>502</v>
       </c>
       <c r="B20" s="44" t="s">
+        <v>516</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>516</v>
+      </c>
+      <c r="D20" s="46" t="s">
         <v>517</v>
-      </c>
-      <c r="C20" s="45" t="s">
-        <v>517</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>518</v>
       </c>
       <c r="E20" s="45"/>
       <c r="F20" s="47"/>
@@ -4167,10 +4164,10 @@
         <v>1</v>
       </c>
       <c r="C22" s="51" t="s">
+        <v>518</v>
+      </c>
+      <c r="D22" s="52" t="s">
         <v>519</v>
-      </c>
-      <c r="D22" s="52" t="s">
-        <v>520</v>
       </c>
       <c r="E22" s="53"/>
       <c r="F22" s="54"/>
@@ -4184,10 +4181,10 @@
         <v>2</v>
       </c>
       <c r="C23" s="51" t="s">
+        <v>520</v>
+      </c>
+      <c r="D23" s="50" t="s">
         <v>521</v>
-      </c>
-      <c r="D23" s="50" t="s">
-        <v>522</v>
       </c>
       <c r="E23" s="53"/>
       <c r="F23" s="54"/>
@@ -4201,10 +4198,10 @@
         <v>3</v>
       </c>
       <c r="C24" s="51" t="s">
+        <v>522</v>
+      </c>
+      <c r="D24" s="50" t="s">
         <v>523</v>
-      </c>
-      <c r="D24" s="50" t="s">
-        <v>524</v>
       </c>
       <c r="E24" s="53"/>
       <c r="F24" s="54"/>
@@ -4218,10 +4215,10 @@
         <v>4</v>
       </c>
       <c r="C25" s="51" t="s">
+        <v>524</v>
+      </c>
+      <c r="D25" s="50" t="s">
         <v>525</v>
-      </c>
-      <c r="D25" s="50" t="s">
-        <v>526</v>
       </c>
       <c r="E25" s="53"/>
       <c r="F25" s="54"/>
@@ -4235,10 +4232,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="51" t="s">
+        <v>526</v>
+      </c>
+      <c r="D26" s="50" t="s">
         <v>527</v>
-      </c>
-      <c r="D26" s="50" t="s">
-        <v>528</v>
       </c>
       <c r="E26" s="53"/>
       <c r="F26" s="54"/>
@@ -4252,10 +4249,10 @@
         <v>6</v>
       </c>
       <c r="C27" s="51" t="s">
+        <v>528</v>
+      </c>
+      <c r="D27" s="50" t="s">
         <v>529</v>
-      </c>
-      <c r="D27" s="50" t="s">
-        <v>530</v>
       </c>
       <c r="E27" s="53"/>
       <c r="F27" s="54"/>
@@ -4269,10 +4266,10 @@
         <v>7</v>
       </c>
       <c r="C28" s="51" t="s">
+        <v>530</v>
+      </c>
+      <c r="D28" s="50" t="s">
         <v>531</v>
-      </c>
-      <c r="D28" s="50" t="s">
-        <v>532</v>
       </c>
       <c r="E28" s="53"/>
       <c r="F28" s="54"/>
@@ -4286,10 +4283,10 @@
         <v>8</v>
       </c>
       <c r="C29" s="51" t="s">
+        <v>532</v>
+      </c>
+      <c r="D29" s="50" t="s">
         <v>533</v>
-      </c>
-      <c r="D29" s="50" t="s">
-        <v>534</v>
       </c>
       <c r="E29" s="53"/>
       <c r="F29" s="54"/>
@@ -4303,10 +4300,10 @@
         <v>9</v>
       </c>
       <c r="C30" s="51" t="s">
+        <v>534</v>
+      </c>
+      <c r="D30" s="50" t="s">
         <v>535</v>
-      </c>
-      <c r="D30" s="50" t="s">
-        <v>536</v>
       </c>
       <c r="E30" s="53"/>
       <c r="F30" s="54"/>
@@ -4323,7 +4320,7 @@
         <v>337</v>
       </c>
       <c r="D31" s="50" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E31" s="53"/>
       <c r="F31" s="54"/>
@@ -4337,10 +4334,10 @@
         <v>11</v>
       </c>
       <c r="C32" s="51" t="s">
+        <v>537</v>
+      </c>
+      <c r="D32" s="50" t="s">
         <v>538</v>
-      </c>
-      <c r="D32" s="50" t="s">
-        <v>539</v>
       </c>
       <c r="E32" s="53"/>
       <c r="F32" s="54"/>
@@ -4354,10 +4351,10 @@
         <v>12</v>
       </c>
       <c r="C33" s="51" t="s">
+        <v>539</v>
+      </c>
+      <c r="D33" s="50" t="s">
         <v>540</v>
-      </c>
-      <c r="D33" s="50" t="s">
-        <v>541</v>
       </c>
       <c r="E33" s="53"/>
       <c r="F33" s="54"/>
@@ -4371,10 +4368,10 @@
         <v>13</v>
       </c>
       <c r="C34" s="51" t="s">
+        <v>541</v>
+      </c>
+      <c r="D34" s="50" t="s">
         <v>542</v>
-      </c>
-      <c r="D34" s="50" t="s">
-        <v>543</v>
       </c>
       <c r="E34" s="53"/>
       <c r="F34" s="54"/>
@@ -4388,10 +4385,10 @@
         <v>14</v>
       </c>
       <c r="C35" s="51" t="s">
+        <v>543</v>
+      </c>
+      <c r="D35" s="50" t="s">
         <v>544</v>
-      </c>
-      <c r="D35" s="50" t="s">
-        <v>545</v>
       </c>
       <c r="E35" s="53"/>
       <c r="F35" s="54"/>
@@ -4405,10 +4402,10 @@
         <v>66</v>
       </c>
       <c r="C36" s="51" t="s">
+        <v>545</v>
+      </c>
+      <c r="D36" s="50" t="s">
         <v>546</v>
-      </c>
-      <c r="D36" s="50" t="s">
-        <v>547</v>
       </c>
       <c r="E36" s="53"/>
       <c r="F36" s="54"/>
@@ -4422,10 +4419,10 @@
         <v>88</v>
       </c>
       <c r="C37" s="51" t="s">
-        <v>548</v>
+        <v>633</v>
       </c>
       <c r="D37" s="50" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E37" s="53"/>
       <c r="F37" s="54"/>
@@ -4442,16 +4439,16 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B39" s="4">
         <v>1</v>
       </c>
       <c r="C39" s="42" t="s">
+        <v>518</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>519</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>520</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="6"/>
@@ -4459,16 +4456,16 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B40" s="4">
         <v>2</v>
       </c>
       <c r="C40" s="42" t="s">
+        <v>520</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>521</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>522</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="6"/>
@@ -4476,16 +4473,16 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B41" s="4">
         <v>3</v>
       </c>
       <c r="C41" s="42" t="s">
+        <v>522</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>523</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>524</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="6"/>
@@ -4493,16 +4490,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B42" s="4">
         <v>4</v>
       </c>
       <c r="C42" s="42" t="s">
+        <v>524</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>525</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>526</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="6"/>
@@ -4510,16 +4507,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B43" s="4">
         <v>5</v>
       </c>
       <c r="C43" s="42" t="s">
+        <v>526</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>527</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>528</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="6"/>
@@ -4527,16 +4524,16 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B44" s="4">
         <v>6</v>
       </c>
       <c r="C44" s="42" t="s">
+        <v>528</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>529</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>530</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="6"/>
@@ -4544,16 +4541,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B45" s="4">
         <v>7</v>
       </c>
       <c r="C45" s="42" t="s">
+        <v>530</v>
+      </c>
+      <c r="D45" s="4" t="s">
         <v>531</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>532</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="6"/>
@@ -4561,16 +4558,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B46" s="4">
         <v>8</v>
       </c>
       <c r="C46" s="42" t="s">
+        <v>532</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>533</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>534</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="6"/>
@@ -4578,16 +4575,16 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B47" s="4">
         <v>9</v>
       </c>
       <c r="C47" s="42" t="s">
+        <v>534</v>
+      </c>
+      <c r="D47" s="4" t="s">
         <v>535</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>536</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="6"/>
@@ -4595,7 +4592,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B48" s="4">
         <v>10</v>
@@ -4604,7 +4601,7 @@
         <v>337</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="6"/>
@@ -4612,16 +4609,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B49" s="4">
         <v>11</v>
       </c>
       <c r="C49" s="42" t="s">
+        <v>537</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>538</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>539</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="6"/>
@@ -4629,16 +4626,16 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B50" s="4">
         <v>12</v>
       </c>
       <c r="C50" s="42" t="s">
+        <v>539</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>540</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>541</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="6"/>
@@ -4646,16 +4643,16 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B51" s="4">
         <v>13</v>
       </c>
       <c r="C51" s="42" t="s">
+        <v>541</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>542</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>543</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="6"/>
@@ -4663,16 +4660,16 @@
     </row>
     <row r="52" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B52" s="4">
         <v>14</v>
       </c>
       <c r="C52" s="42" t="s">
+        <v>543</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>544</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>545</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="6"/>
@@ -4680,16 +4677,16 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B53" s="4">
         <v>66</v>
       </c>
       <c r="C53" s="42" t="s">
+        <v>545</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>546</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>547</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="6"/>
@@ -4697,16 +4694,16 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B54" s="4">
         <v>88</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>548</v>
+        <v>633</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="6"/>
@@ -4732,7 +4729,7 @@
         <v>338</v>
       </c>
       <c r="D56" s="42" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="6"/>
@@ -4749,7 +4746,7 @@
         <v>339</v>
       </c>
       <c r="D57" s="52" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E57" s="53"/>
       <c r="F57" s="54"/>
@@ -4766,7 +4763,7 @@
         <v>340</v>
       </c>
       <c r="D58" s="52" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E58" s="53"/>
       <c r="F58" s="54"/>
@@ -4777,13 +4774,13 @@
         <v>36</v>
       </c>
       <c r="B59" s="46" t="s">
+        <v>552</v>
+      </c>
+      <c r="C59" s="45" t="s">
+        <v>553</v>
+      </c>
+      <c r="D59" s="44" t="s">
         <v>554</v>
-      </c>
-      <c r="C59" s="45" t="s">
-        <v>555</v>
-      </c>
-      <c r="D59" s="44" t="s">
-        <v>556</v>
       </c>
       <c r="E59" s="45"/>
       <c r="F59" s="47"/>
@@ -4794,13 +4791,13 @@
         <v>36</v>
       </c>
       <c r="B60" s="46" t="s">
+        <v>555</v>
+      </c>
+      <c r="C60" s="45" t="s">
+        <v>556</v>
+      </c>
+      <c r="D60" s="44" t="s">
         <v>557</v>
-      </c>
-      <c r="C60" s="45" t="s">
-        <v>558</v>
-      </c>
-      <c r="D60" s="44" t="s">
-        <v>559</v>
       </c>
       <c r="E60" s="45"/>
       <c r="F60" s="47"/>
@@ -4811,13 +4808,13 @@
         <v>36</v>
       </c>
       <c r="B61" s="46" t="s">
+        <v>558</v>
+      </c>
+      <c r="C61" s="45" t="s">
+        <v>559</v>
+      </c>
+      <c r="D61" s="44" t="s">
         <v>560</v>
-      </c>
-      <c r="C61" s="45" t="s">
-        <v>561</v>
-      </c>
-      <c r="D61" s="44" t="s">
-        <v>562</v>
       </c>
       <c r="E61" s="45"/>
       <c r="F61" s="47"/>
@@ -4828,13 +4825,13 @@
         <v>36</v>
       </c>
       <c r="B62" s="46" t="s">
+        <v>561</v>
+      </c>
+      <c r="C62" s="45" t="s">
+        <v>562</v>
+      </c>
+      <c r="D62" s="44" t="s">
         <v>563</v>
-      </c>
-      <c r="C62" s="45" t="s">
-        <v>564</v>
-      </c>
-      <c r="D62" s="44" t="s">
-        <v>565</v>
       </c>
       <c r="E62" s="45"/>
       <c r="F62" s="47"/>
@@ -4845,13 +4842,13 @@
         <v>36</v>
       </c>
       <c r="B63" s="46" t="s">
+        <v>564</v>
+      </c>
+      <c r="C63" s="45" t="s">
+        <v>565</v>
+      </c>
+      <c r="D63" s="44" t="s">
         <v>566</v>
-      </c>
-      <c r="C63" s="45" t="s">
-        <v>567</v>
-      </c>
-      <c r="D63" s="44" t="s">
-        <v>568</v>
       </c>
       <c r="E63" s="45"/>
       <c r="F63" s="47"/>
@@ -4862,13 +4859,13 @@
         <v>36</v>
       </c>
       <c r="B64" s="46" t="s">
+        <v>567</v>
+      </c>
+      <c r="C64" s="45" t="s">
+        <v>568</v>
+      </c>
+      <c r="D64" s="44" t="s">
         <v>569</v>
-      </c>
-      <c r="C64" s="45" t="s">
-        <v>570</v>
-      </c>
-      <c r="D64" s="44" t="s">
-        <v>571</v>
       </c>
       <c r="E64" s="45"/>
       <c r="F64" s="47"/>
@@ -4879,13 +4876,13 @@
         <v>36</v>
       </c>
       <c r="B65" s="46" t="s">
+        <v>570</v>
+      </c>
+      <c r="C65" s="45" t="s">
+        <v>571</v>
+      </c>
+      <c r="D65" s="44" t="s">
         <v>572</v>
-      </c>
-      <c r="C65" s="45" t="s">
-        <v>573</v>
-      </c>
-      <c r="D65" s="44" t="s">
-        <v>574</v>
       </c>
       <c r="E65" s="45"/>
       <c r="F65" s="47"/>
@@ -4896,13 +4893,13 @@
         <v>36</v>
       </c>
       <c r="B66" s="46" t="s">
+        <v>573</v>
+      </c>
+      <c r="C66" s="45" t="s">
+        <v>574</v>
+      </c>
+      <c r="D66" s="44" t="s">
         <v>575</v>
-      </c>
-      <c r="C66" s="45" t="s">
-        <v>576</v>
-      </c>
-      <c r="D66" s="44" t="s">
-        <v>577</v>
       </c>
       <c r="E66" s="45"/>
       <c r="F66" s="47"/>
@@ -4913,13 +4910,13 @@
         <v>36</v>
       </c>
       <c r="B67" s="46" t="s">
+        <v>576</v>
+      </c>
+      <c r="C67" s="45" t="s">
+        <v>577</v>
+      </c>
+      <c r="D67" s="44" t="s">
         <v>578</v>
-      </c>
-      <c r="C67" s="45" t="s">
-        <v>579</v>
-      </c>
-      <c r="D67" s="44" t="s">
-        <v>580</v>
       </c>
       <c r="E67" s="45"/>
       <c r="F67" s="47"/>
@@ -4930,13 +4927,13 @@
         <v>36</v>
       </c>
       <c r="B68" s="46" t="s">
-        <v>581</v>
+        <v>632</v>
       </c>
       <c r="C68" s="45" t="s">
-        <v>548</v>
+        <v>633</v>
       </c>
       <c r="D68" s="44" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E68" s="45"/>
       <c r="F68" s="47"/>
@@ -4947,13 +4944,13 @@
         <v>36</v>
       </c>
       <c r="B69" s="46" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C69" s="45" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="D69" s="44" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E69" s="45"/>
       <c r="F69" s="47"/>
@@ -4979,7 +4976,7 @@
         <v>389</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="6"/>
@@ -4996,7 +4993,7 @@
         <v>390</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="6"/>
@@ -5004,7 +5001,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>389</v>
@@ -5013,7 +5010,7 @@
         <v>389</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="6"/>
@@ -5021,7 +5018,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>390</v>
@@ -5030,7 +5027,7 @@
         <v>390</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="6"/>
@@ -5047,7 +5044,7 @@
         <v>341</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="6"/>
@@ -5064,7 +5061,7 @@
         <v>342</v>
       </c>
       <c r="D76" s="56" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="6"/>
@@ -5081,7 +5078,7 @@
         <v>343</v>
       </c>
       <c r="D77" s="56" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="6"/>
@@ -5098,7 +5095,7 @@
         <v>344</v>
       </c>
       <c r="D78" s="42" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="6"/>
@@ -5115,7 +5112,7 @@
         <v>345</v>
       </c>
       <c r="D79" s="42" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="6"/>
@@ -5132,7 +5129,7 @@
         <v>346</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="6"/>
@@ -5149,7 +5146,7 @@
         <v>347</v>
       </c>
       <c r="D81" s="42" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="6"/>
@@ -5166,7 +5163,7 @@
         <v>348</v>
       </c>
       <c r="D82" s="42" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="6"/>
@@ -5177,13 +5174,13 @@
         <v>40</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="6"/>
@@ -5200,7 +5197,7 @@
         <v>333</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="6"/>
@@ -5217,7 +5214,7 @@
         <v>349</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="E85" s="5"/>
       <c r="F85" s="6"/>
@@ -5234,7 +5231,7 @@
         <v>350</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E86" s="5"/>
       <c r="F86" s="6"/>
@@ -5251,7 +5248,7 @@
         <v>351</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="E87" s="7"/>
       <c r="G87" s="6"/>
@@ -5262,31 +5259,31 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>622</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>625</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>626</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>628</v>
       </c>
       <c r="E89" s="7"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E90" s="7"/>
     </row>
@@ -5429,7 +5426,7 @@
         <v>326</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>196</v>
@@ -5448,7 +5445,7 @@
         <v>327</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>222</v>
@@ -5467,7 +5464,7 @@
         <v>328</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>248</v>
@@ -5486,7 +5483,7 @@
         <v>85</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>57</v>
@@ -5505,7 +5502,7 @@
         <v>325</v>
       </c>
       <c r="D105" s="16" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="E105" s="16" t="s">
         <v>57</v>
@@ -5524,7 +5521,7 @@
         <v>329</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>272</v>
@@ -5543,7 +5540,7 @@
         <v>330</v>
       </c>
       <c r="D107" s="16" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>298</v>
@@ -5562,7 +5559,7 @@
         <v>113</v>
       </c>
       <c r="D108" s="16" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>112</v>
@@ -5581,7 +5578,7 @@
         <v>141</v>
       </c>
       <c r="D109" s="16" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>140</v>
@@ -5600,7 +5597,7 @@
         <v>170</v>
       </c>
       <c r="D110" s="16" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
tz: update some forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Tanzania/tz_sch_sth_impact_202311_1_school.xlsx
+++ b/SCH-STH/Impact assessments/Tanzania/tz_sch_sth_impact_202311_1_school.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Tanzania\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4B99CD-2D74-4B77-A257-CAC55183ECD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F3F345-B2AF-4FAC-B787-8090DA4D3B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3703" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3703" uniqueCount="650">
   <si>
     <t>type</t>
   </si>
@@ -1388,9 +1388,6 @@
     <t>How long does it take to go there, get handwashing water, and come back?</t>
   </si>
   <si>
-    <t>Inachukua muda gani kupata maji ya kunawa na kurudi?</t>
-  </si>
-  <si>
     <t>w_regi_class_IV</t>
   </si>
   <si>
@@ -1544,16 +1541,7 @@
     <t>Zaidi ya miezi 6</t>
   </si>
   <si>
-    <t>Piped water into dwelling</t>
-  </si>
-  <si>
-    <t>Maji ya bomba ndani ya nyumba</t>
-  </si>
-  <si>
     <t>Piped water to compound, yard, or plot</t>
-  </si>
-  <si>
-    <t>Maji ya bomba ndani ya eneo la kiwanja cha nyumba</t>
   </si>
   <si>
     <t>Piped water to neighbour</t>
@@ -1913,9 +1901,6 @@
     <t>Alitoa</t>
   </si>
   <si>
-    <t>Imekataa</t>
-  </si>
-  <si>
     <t>select_one consent</t>
   </si>
   <si>
@@ -1970,9 +1955,6 @@
     <t>Kwa mfano, shimo limefunikwa?</t>
   </si>
   <si>
-    <t>Mtazamaji: Ni vifaa gani vya kunawia mikono vinapatikana?</t>
-  </si>
-  <si>
     <t>Je, ni vifaa gani unaweza kuona angalau mita 3 kutoka kwenye vyoo wakati wa uchunguzi?</t>
   </si>
   <si>
@@ -2027,12 +2009,6 @@
     <t>Chagua jibu sahihi, kama chanzo cha maji kiko ndani ya shule chagua 0</t>
   </si>
   <si>
-    <t>1.Chini ya dakika 30 kwenda na kurudi kutoka shuleni</t>
-  </si>
-  <si>
-    <t>2. More than 30 minutes to and from school</t>
-  </si>
-  <si>
     <t>1. Less than 30 minutes round trip from school</t>
   </si>
   <si>
@@ -2054,10 +2030,22 @@
     <t>Pond/Lake/Sea/River</t>
   </si>
   <si>
-    <t>(2024 Jan) - 1. SCH/STH – School/Location V4</t>
-  </si>
-  <si>
-    <t>tz_sch_sth_impact_202311_1_school_v4</t>
+    <t>Amekataa</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Inachukua muda gani jumla kwenda, kusubiri, kupata maji ya kunawa na kurudi?</t>
+  </si>
+  <si>
+    <t>Mtazamaji: Ni vifaa gani vya kunawia mikono vinapatikana angalau mita 3 kutoka kwenye vyoo?</t>
+  </si>
+  <si>
+    <t>(2024 Jan) - 1. SCH/STH – School/Location V4.1</t>
+  </si>
+  <si>
+    <t>tz_sch_sth_impact_202311_1_school_v4_1</t>
   </si>
 </sst>
 </file>
@@ -2129,7 +2117,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2181,6 +2169,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2253,7 +2253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2402,11 +2402,29 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2764,10 +2782,10 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2939,7 +2957,7 @@
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="35" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="F5" s="35"/>
       <c r="G5" s="25"/>
@@ -3047,17 +3065,17 @@
     </row>
     <row r="9" spans="1:15" s="28" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="35" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="F9" s="35"/>
       <c r="G9" s="25"/>
@@ -3077,14 +3095,14 @@
         <v>24</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="35" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="F10" s="35"/>
       <c r="G10" s="25"/>
@@ -3092,7 +3110,7 @@
       <c r="I10" s="27"/>
       <c r="J10" s="35"/>
       <c r="K10" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L10" s="25"/>
       <c r="M10" s="25" t="s">
@@ -3106,32 +3124,32 @@
         <v>24</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="J11" s="35" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L11" s="25"/>
       <c r="M11" s="25" t="s">
@@ -3145,13 +3163,13 @@
         <v>332</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>408</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>409</v>
@@ -3164,7 +3182,7 @@
       <c r="I12" s="27"/>
       <c r="J12" s="35"/>
       <c r="K12" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L12" s="25"/>
       <c r="M12" s="25" t="s">
@@ -3178,13 +3196,13 @@
         <v>332</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>411</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>412</v>
@@ -3197,7 +3215,7 @@
       <c r="I13" s="27"/>
       <c r="J13" s="35"/>
       <c r="K13" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25" t="s">
@@ -3211,13 +3229,13 @@
         <v>332</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>413</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="E14" s="35" t="s">
         <v>414</v>
@@ -3230,7 +3248,7 @@
       <c r="I14" s="27"/>
       <c r="J14" s="35"/>
       <c r="K14" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L14" s="25"/>
       <c r="M14" s="25" t="s">
@@ -3244,7 +3262,7 @@
         <v>332</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>415</v>
@@ -3260,7 +3278,7 @@
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="25" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="I15" s="27" t="s">
         <v>419</v>
@@ -3269,7 +3287,7 @@
         <v>420</v>
       </c>
       <c r="K15" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L15" s="25"/>
       <c r="M15" s="25" t="s">
@@ -3283,7 +3301,7 @@
         <v>332</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>421</v>
@@ -3299,7 +3317,7 @@
       </c>
       <c r="G16" s="25"/>
       <c r="H16" s="25" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="I16" s="27" t="s">
         <v>423</v>
@@ -3308,7 +3326,7 @@
         <v>424</v>
       </c>
       <c r="K16" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L16" s="25"/>
       <c r="M16" s="25" t="s">
@@ -3322,7 +3340,7 @@
         <v>332</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>425</v>
@@ -3338,7 +3356,7 @@
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="I17" s="27" t="s">
         <v>427</v>
@@ -3347,7 +3365,7 @@
         <v>428</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25" t="s">
@@ -3364,11 +3382,11 @@
         <v>430</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="35" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="25"/>
@@ -3376,7 +3394,7 @@
       <c r="I18" s="27"/>
       <c r="J18" s="35"/>
       <c r="K18" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25" t="s">
@@ -3387,7 +3405,7 @@
     </row>
     <row r="19" spans="1:15" s="28" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>431</v>
@@ -3405,7 +3423,7 @@
       <c r="I19" s="27"/>
       <c r="J19" s="35"/>
       <c r="K19" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L19" s="25"/>
       <c r="M19" s="25" t="s">
@@ -3438,7 +3456,7 @@
       <c r="I20" s="27"/>
       <c r="J20" s="35"/>
       <c r="K20" s="25" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="L20" s="25"/>
       <c r="M20" s="25" t="s">
@@ -3461,17 +3479,17 @@
         <v>440</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
       <c r="I21" s="27"/>
       <c r="J21" s="35"/>
       <c r="K21" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25" t="s">
@@ -3482,7 +3500,7 @@
     </row>
     <row r="22" spans="1:15" s="28" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>441</v>
@@ -3500,7 +3518,7 @@
       <c r="I22" s="27"/>
       <c r="J22" s="35"/>
       <c r="K22" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L22" s="25"/>
       <c r="M22" s="25" t="s">
@@ -3531,7 +3549,7 @@
       <c r="I23" s="27"/>
       <c r="J23" s="35"/>
       <c r="K23" s="25" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="L23" s="25"/>
       <c r="M23" s="25" t="s">
@@ -3553,18 +3571,18 @@
       <c r="D24" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="E24" s="35" t="s">
-        <v>450</v>
+      <c r="E24" s="65" t="s">
+        <v>646</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
       <c r="I24" s="27"/>
       <c r="J24" s="35"/>
       <c r="K24" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25" t="s">
@@ -3581,23 +3599,23 @@
         <v>17</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>372</v>
       </c>
       <c r="E25" s="35" t="s">
+        <v>457</v>
+      </c>
+      <c r="F25" s="35" t="s">
         <v>458</v>
-      </c>
-      <c r="F25" s="35" t="s">
-        <v>459</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
       <c r="I25" s="27"/>
       <c r="J25" s="35"/>
       <c r="K25" s="25" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25" t="s">
@@ -3608,29 +3626,29 @@
     </row>
     <row r="26" spans="1:15" s="14" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
+        <v>459</v>
+      </c>
+      <c r="B26" s="26" t="s">
         <v>460</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="C26" s="32" t="s">
         <v>461</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="D26" s="32" t="s">
         <v>462</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="E26" s="36" t="s">
+        <v>640</v>
+      </c>
+      <c r="F26" s="36" t="s">
         <v>463</v>
-      </c>
-      <c r="E26" s="36" t="s">
-        <v>648</v>
-      </c>
-      <c r="F26" s="36" t="s">
-        <v>464</v>
       </c>
       <c r="G26" s="33"/>
       <c r="H26" s="33"/>
       <c r="I26" s="32"/>
       <c r="J26" s="36"/>
       <c r="K26" s="25" t="s">
-        <v>649</v>
+        <v>641</v>
       </c>
       <c r="L26" s="33"/>
       <c r="M26" s="25" t="s">
@@ -3644,16 +3662,16 @@
         <v>24</v>
       </c>
       <c r="B27" s="26" t="s">
+        <v>464</v>
+      </c>
+      <c r="C27" s="32" t="s">
         <v>465</v>
-      </c>
-      <c r="C27" s="32" t="s">
-        <v>466</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>436</v>
       </c>
       <c r="E27" s="36" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F27" s="36" t="s">
         <v>438</v>
@@ -3663,7 +3681,7 @@
       <c r="I27" s="32"/>
       <c r="J27" s="36"/>
       <c r="K27" s="25" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="L27" s="33"/>
       <c r="M27" s="25" t="s">
@@ -3680,11 +3698,11 @@
         <v>18</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D28" s="32"/>
       <c r="E28" s="36" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F28" s="36"/>
       <c r="G28" s="33"/>
@@ -3692,7 +3710,7 @@
       <c r="I28" s="32"/>
       <c r="J28" s="36"/>
       <c r="K28" s="25" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="L28" s="33"/>
       <c r="M28" s="25" t="s">
@@ -3706,26 +3724,26 @@
         <v>24</v>
       </c>
       <c r="B29" s="26" t="s">
+        <v>469</v>
+      </c>
+      <c r="C29" s="27" t="s">
         <v>470</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="D29" s="27" t="s">
+        <v>605</v>
+      </c>
+      <c r="E29" s="35" t="s">
         <v>471</v>
       </c>
-      <c r="D29" s="27" t="s">
-        <v>610</v>
-      </c>
-      <c r="E29" s="35" t="s">
+      <c r="F29" s="35" t="s">
         <v>472</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>473</v>
       </c>
       <c r="G29" s="25"/>
       <c r="H29" s="25"/>
       <c r="I29" s="27"/>
       <c r="J29" s="35"/>
       <c r="K29" s="25" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="L29" s="25"/>
       <c r="M29" s="25" t="s">
@@ -3746,7 +3764,7 @@
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="35" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="F30" s="35"/>
       <c r="G30" s="25"/>
@@ -3754,7 +3772,7 @@
       <c r="I30" s="27"/>
       <c r="J30" s="35"/>
       <c r="K30" s="25" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="L30" s="25"/>
       <c r="M30" s="25" t="s">
@@ -3777,17 +3795,17 @@
         <v>373</v>
       </c>
       <c r="E31" s="35" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="F31" s="35" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="G31" s="33"/>
       <c r="H31" s="33"/>
       <c r="I31" s="32"/>
       <c r="J31" s="36"/>
       <c r="K31" s="25" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="L31" s="33"/>
       <c r="M31" s="25" t="s">
@@ -3809,18 +3827,18 @@
       <c r="D32" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="E32" s="35" t="s">
-        <v>624</v>
+      <c r="E32" s="65" t="s">
+        <v>647</v>
       </c>
       <c r="F32" s="35" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="G32" s="33"/>
       <c r="H32" s="33"/>
       <c r="I32" s="32"/>
       <c r="J32" s="36"/>
       <c r="K32" s="25" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="L32" s="33"/>
       <c r="M32" s="25" t="s">
@@ -3841,7 +3859,7 @@
       </c>
       <c r="D33" s="32"/>
       <c r="E33" s="36" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="F33" s="36"/>
       <c r="G33" s="33"/>
@@ -3907,8 +3925,8 @@
   <dimension ref="A1:H565"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C72" sqref="C72"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3960,7 +3978,7 @@
         <v>334</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
@@ -3977,7 +3995,7 @@
         <v>335</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="6"/>
@@ -3994,7 +4012,7 @@
         <v>334</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
@@ -4011,7 +4029,7 @@
         <v>335</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
@@ -4028,7 +4046,7 @@
         <v>336</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
@@ -4045,16 +4063,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
+        <v>476</v>
+      </c>
+      <c r="B8" s="42" t="s">
         <v>477</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="C8" s="43" t="s">
         <v>478</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="D8" s="42" t="s">
         <v>479</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>480</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
@@ -4062,16 +4080,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B9" s="42" t="s">
+        <v>480</v>
+      </c>
+      <c r="C9" s="43" t="s">
         <v>481</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="D9" s="42" t="s">
         <v>482</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>483</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
@@ -4079,16 +4097,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>651</v>
+        <v>643</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>650</v>
+        <v>642</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
@@ -4096,16 +4114,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B11" s="42" t="s">
+        <v>483</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>483</v>
+      </c>
+      <c r="D11" s="42" t="s">
         <v>484</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>484</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>485</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
@@ -4113,7 +4131,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B12" s="44" t="s">
         <v>343</v>
@@ -4122,7 +4140,7 @@
         <v>343</v>
       </c>
       <c r="D12" s="46" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E12" s="45"/>
       <c r="F12" s="47"/>
@@ -4131,7 +4149,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B13" s="46" t="s">
         <v>336</v>
@@ -4140,7 +4158,7 @@
         <v>336</v>
       </c>
       <c r="D13" s="46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E13" s="45"/>
       <c r="F13" s="47"/>
@@ -4149,16 +4167,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B14" s="44" t="s">
+        <v>487</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>487</v>
+      </c>
+      <c r="D14" s="46" t="s">
         <v>488</v>
-      </c>
-      <c r="C14" s="45" t="s">
-        <v>488</v>
-      </c>
-      <c r="D14" s="46" t="s">
-        <v>489</v>
       </c>
       <c r="E14" s="45"/>
       <c r="F14" s="47"/>
@@ -4167,16 +4185,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B15" s="44" t="s">
+        <v>489</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>489</v>
+      </c>
+      <c r="D15" s="46" t="s">
         <v>490</v>
-      </c>
-      <c r="C15" s="45" t="s">
-        <v>490</v>
-      </c>
-      <c r="D15" s="46" t="s">
-        <v>491</v>
       </c>
       <c r="E15" s="45"/>
       <c r="F15" s="47"/>
@@ -4185,16 +4203,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B16" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>491</v>
+      </c>
+      <c r="D16" s="46" t="s">
         <v>492</v>
-      </c>
-      <c r="C16" s="45" t="s">
-        <v>492</v>
-      </c>
-      <c r="D16" s="46" t="s">
-        <v>493</v>
       </c>
       <c r="E16" s="45"/>
       <c r="F16" s="47"/>
@@ -4203,16 +4221,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B17" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>493</v>
+      </c>
+      <c r="D17" s="46" t="s">
         <v>494</v>
-      </c>
-      <c r="C17" s="45" t="s">
-        <v>494</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>495</v>
       </c>
       <c r="E17" s="45"/>
       <c r="F17" s="47"/>
@@ -4221,16 +4239,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B18" s="44" t="s">
+        <v>495</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>495</v>
+      </c>
+      <c r="D18" s="46" t="s">
         <v>496</v>
-      </c>
-      <c r="C18" s="45" t="s">
-        <v>496</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>497</v>
       </c>
       <c r="E18" s="45"/>
       <c r="F18" s="47"/>
@@ -4239,16 +4257,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B19" s="44" t="s">
+        <v>497</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>497</v>
+      </c>
+      <c r="D19" s="46" t="s">
         <v>498</v>
-      </c>
-      <c r="C19" s="45" t="s">
-        <v>498</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>499</v>
       </c>
       <c r="E19" s="45"/>
       <c r="F19" s="47"/>
@@ -4257,16 +4275,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B20" s="44" t="s">
+        <v>499</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>499</v>
+      </c>
+      <c r="D20" s="46" t="s">
         <v>500</v>
-      </c>
-      <c r="C20" s="45" t="s">
-        <v>500</v>
-      </c>
-      <c r="D20" s="46" t="s">
-        <v>501</v>
       </c>
       <c r="E20" s="45"/>
       <c r="F20" s="47"/>
@@ -4290,10 +4308,10 @@
         <v>1</v>
       </c>
       <c r="C22" s="42" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="6"/>
@@ -4307,10 +4325,10 @@
         <v>2</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="6"/>
@@ -4324,10 +4342,10 @@
         <v>3</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="6"/>
@@ -4341,10 +4359,10 @@
         <v>4</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="6"/>
@@ -4358,10 +4376,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
@@ -4375,10 +4393,10 @@
         <v>6</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="6"/>
@@ -4392,10 +4410,10 @@
         <v>7</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="6"/>
@@ -4409,10 +4427,10 @@
         <v>8</v>
       </c>
       <c r="C29" s="42" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="6"/>
@@ -4429,7 +4447,7 @@
         <v>337</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="6"/>
@@ -4443,10 +4461,10 @@
         <v>10</v>
       </c>
       <c r="C31" s="42" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="6"/>
@@ -4460,10 +4478,10 @@
         <v>11</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="6"/>
@@ -4477,10 +4495,10 @@
         <v>12</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
@@ -4494,10 +4512,10 @@
         <v>13</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
@@ -4511,10 +4529,10 @@
         <v>14</v>
       </c>
       <c r="C35" s="56" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -4525,10 +4543,10 @@
         <v>66</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="6"/>
@@ -4542,10 +4560,10 @@
         <v>88</v>
       </c>
       <c r="C37" s="42" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="6"/>
@@ -4560,277 +4578,277 @@
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B39" s="57">
         <v>1</v>
       </c>
-      <c r="C39" s="58" t="s">
-        <v>502</v>
-      </c>
-      <c r="D39" s="57" t="s">
-        <v>503</v>
+      <c r="C39" s="66" t="s">
+        <v>501</v>
+      </c>
+      <c r="D39" s="62" t="s">
+        <v>625</v>
       </c>
       <c r="E39" s="57"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
-    </row>
-    <row r="40" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+    </row>
+    <row r="40" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B40" s="57">
         <v>2</v>
       </c>
-      <c r="C40" s="58" t="s">
-        <v>504</v>
-      </c>
-      <c r="D40" s="57" t="s">
-        <v>505</v>
+      <c r="C40" s="66" t="s">
+        <v>502</v>
+      </c>
+      <c r="D40" s="62" t="s">
+        <v>503</v>
       </c>
       <c r="E40" s="57"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="59"/>
-    </row>
-    <row r="41" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+    </row>
+    <row r="41" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B41" s="57">
         <v>3</v>
       </c>
-      <c r="C41" s="58" t="s">
-        <v>506</v>
-      </c>
-      <c r="D41" s="57" t="s">
-        <v>507</v>
+      <c r="C41" s="66" t="s">
+        <v>504</v>
+      </c>
+      <c r="D41" s="62" t="s">
+        <v>505</v>
       </c>
       <c r="E41" s="57"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
-    </row>
-    <row r="42" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+    </row>
+    <row r="42" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B42" s="57">
         <v>4</v>
       </c>
-      <c r="C42" s="58" t="s">
-        <v>508</v>
-      </c>
-      <c r="D42" s="57" t="s">
-        <v>509</v>
+      <c r="C42" s="66" t="s">
+        <v>506</v>
+      </c>
+      <c r="D42" s="62" t="s">
+        <v>507</v>
       </c>
       <c r="E42" s="57"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-    </row>
-    <row r="43" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+    </row>
+    <row r="43" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B43" s="57">
         <v>5</v>
       </c>
-      <c r="C43" s="58" t="s">
-        <v>510</v>
-      </c>
-      <c r="D43" s="57" t="s">
-        <v>511</v>
+      <c r="C43" s="66" t="s">
+        <v>508</v>
+      </c>
+      <c r="D43" s="62" t="s">
+        <v>509</v>
       </c>
       <c r="E43" s="57"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="59"/>
-    </row>
-    <row r="44" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+    </row>
+    <row r="44" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B44" s="57">
         <v>6</v>
       </c>
-      <c r="C44" s="58" t="s">
-        <v>512</v>
-      </c>
-      <c r="D44" s="57" t="s">
-        <v>513</v>
+      <c r="C44" s="66" t="s">
+        <v>510</v>
+      </c>
+      <c r="D44" s="62" t="s">
+        <v>511</v>
       </c>
       <c r="E44" s="57"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-    </row>
-    <row r="45" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F44" s="58"/>
+      <c r="G44" s="58"/>
+    </row>
+    <row r="45" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B45" s="57">
         <v>7</v>
       </c>
-      <c r="C45" s="58" t="s">
-        <v>514</v>
-      </c>
-      <c r="D45" s="57" t="s">
-        <v>515</v>
+      <c r="C45" s="66" t="s">
+        <v>512</v>
+      </c>
+      <c r="D45" s="62" t="s">
+        <v>513</v>
       </c>
       <c r="E45" s="57"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="59"/>
-    </row>
-    <row r="46" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+    </row>
+    <row r="46" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B46" s="57">
         <v>8</v>
       </c>
-      <c r="C46" s="58" t="s">
-        <v>516</v>
-      </c>
-      <c r="D46" s="57" t="s">
-        <v>517</v>
+      <c r="C46" s="66" t="s">
+        <v>514</v>
+      </c>
+      <c r="D46" s="62" t="s">
+        <v>515</v>
       </c>
       <c r="E46" s="57"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="59"/>
-    </row>
-    <row r="47" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+    </row>
+    <row r="47" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B47" s="57">
         <v>9</v>
       </c>
-      <c r="C47" s="58" t="s">
-        <v>518</v>
-      </c>
-      <c r="D47" s="57" t="s">
-        <v>519</v>
+      <c r="C47" s="66" t="s">
+        <v>337</v>
+      </c>
+      <c r="D47" s="62" t="s">
+        <v>516</v>
       </c>
       <c r="E47" s="57"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="59"/>
-    </row>
-    <row r="48" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+    </row>
+    <row r="48" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B48" s="57">
         <v>10</v>
       </c>
-      <c r="C48" s="58" t="s">
-        <v>337</v>
-      </c>
-      <c r="D48" s="57" t="s">
-        <v>520</v>
+      <c r="C48" s="66" t="s">
+        <v>517</v>
+      </c>
+      <c r="D48" s="62" t="s">
+        <v>518</v>
       </c>
       <c r="E48" s="57"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="59"/>
-    </row>
-    <row r="49" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+    </row>
+    <row r="49" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B49" s="57">
         <v>11</v>
       </c>
-      <c r="C49" s="58" t="s">
-        <v>521</v>
-      </c>
-      <c r="D49" s="57" t="s">
-        <v>522</v>
+      <c r="C49" s="66" t="s">
+        <v>519</v>
+      </c>
+      <c r="D49" s="62" t="s">
+        <v>520</v>
       </c>
       <c r="E49" s="57"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="59"/>
-    </row>
-    <row r="50" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+    </row>
+    <row r="50" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B50" s="57">
         <v>12</v>
       </c>
-      <c r="C50" s="58" t="s">
-        <v>523</v>
-      </c>
-      <c r="D50" s="57" t="s">
-        <v>524</v>
+      <c r="C50" s="66" t="s">
+        <v>521</v>
+      </c>
+      <c r="D50" s="62" t="s">
+        <v>522</v>
       </c>
       <c r="E50" s="57"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="59"/>
-    </row>
-    <row r="51" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
+    </row>
+    <row r="51" spans="1:7" s="59" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A51" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B51" s="57">
         <v>13</v>
       </c>
-      <c r="C51" s="58" t="s">
-        <v>525</v>
-      </c>
-      <c r="D51" s="57" t="s">
-        <v>526</v>
+      <c r="C51" s="66" t="s">
+        <v>523</v>
+      </c>
+      <c r="D51" s="62" t="s">
+        <v>524</v>
       </c>
       <c r="E51" s="57"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="59"/>
-    </row>
-    <row r="52" spans="1:7" s="60" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="F51" s="58"/>
+      <c r="G51" s="58"/>
+    </row>
+    <row r="52" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B52" s="57">
         <v>14</v>
       </c>
-      <c r="C52" s="58" t="s">
-        <v>527</v>
-      </c>
-      <c r="D52" s="57" t="s">
+      <c r="C52" s="64" t="s">
+        <v>627</v>
+      </c>
+      <c r="D52" s="64" t="s">
+        <v>626</v>
+      </c>
+      <c r="E52" s="57"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
+    </row>
+    <row r="53" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="57" t="s">
         <v>528</v>
-      </c>
-      <c r="E52" s="57"/>
-      <c r="F52" s="59"/>
-      <c r="G52" s="59"/>
-    </row>
-    <row r="53" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="57" t="s">
-        <v>532</v>
       </c>
       <c r="B53" s="57">
         <v>66</v>
       </c>
-      <c r="C53" s="58" t="s">
-        <v>529</v>
-      </c>
-      <c r="D53" s="57" t="s">
-        <v>530</v>
+      <c r="C53" s="66" t="s">
+        <v>525</v>
+      </c>
+      <c r="D53" s="62" t="s">
+        <v>526</v>
       </c>
       <c r="E53" s="57"/>
-      <c r="F53" s="59"/>
-      <c r="G53" s="59"/>
-    </row>
-    <row r="54" spans="1:7" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+    </row>
+    <row r="54" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="57" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B54" s="57">
         <v>88</v>
       </c>
-      <c r="C54" s="58" t="s">
-        <v>634</v>
-      </c>
-      <c r="D54" s="57" t="s">
-        <v>531</v>
+      <c r="C54" s="66" t="s">
+        <v>628</v>
+      </c>
+      <c r="D54" s="62" t="s">
+        <v>527</v>
       </c>
       <c r="E54" s="57"/>
-      <c r="F54" s="59"/>
-      <c r="G54" s="59"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
@@ -4852,7 +4870,7 @@
         <v>338</v>
       </c>
       <c r="D56" s="42" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="6"/>
@@ -4869,7 +4887,7 @@
         <v>339</v>
       </c>
       <c r="D57" s="51" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="E57" s="52"/>
       <c r="F57" s="53"/>
@@ -4886,7 +4904,7 @@
         <v>340</v>
       </c>
       <c r="D58" s="51" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="E58" s="52"/>
       <c r="F58" s="53"/>
@@ -4897,13 +4915,13 @@
         <v>36</v>
       </c>
       <c r="B59" s="46" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C59" s="45" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="D59" s="44" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="E59" s="45"/>
       <c r="F59" s="47"/>
@@ -4914,13 +4932,13 @@
         <v>36</v>
       </c>
       <c r="B60" s="46" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="C60" s="45" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="D60" s="44" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="E60" s="45"/>
       <c r="F60" s="47"/>
@@ -4931,13 +4949,13 @@
         <v>36</v>
       </c>
       <c r="B61" s="46" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="C61" s="45" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D61" s="44" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="E61" s="45"/>
       <c r="F61" s="47"/>
@@ -4948,13 +4966,13 @@
         <v>36</v>
       </c>
       <c r="B62" s="46" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C62" s="45" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D62" s="44" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="E62" s="45"/>
       <c r="F62" s="47"/>
@@ -4965,13 +4983,13 @@
         <v>36</v>
       </c>
       <c r="B63" s="46" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C63" s="45" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="D63" s="44" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="E63" s="45"/>
       <c r="F63" s="47"/>
@@ -4982,13 +5000,13 @@
         <v>36</v>
       </c>
       <c r="B64" s="46" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C64" s="45" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="D64" s="44" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="E64" s="45"/>
       <c r="F64" s="47"/>
@@ -4999,13 +5017,13 @@
         <v>36</v>
       </c>
       <c r="B65" s="46" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D65" s="44" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="E65" s="45"/>
       <c r="F65" s="47"/>
@@ -5016,13 +5034,13 @@
         <v>36</v>
       </c>
       <c r="B66" s="46" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C66" s="45" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D66" s="44" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="E66" s="45"/>
       <c r="F66" s="47"/>
@@ -5033,13 +5051,13 @@
         <v>36</v>
       </c>
       <c r="B67" s="46" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="C67" s="45" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="D67" s="44" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="E67" s="45"/>
       <c r="F67" s="47"/>
@@ -5050,13 +5068,13 @@
         <v>36</v>
       </c>
       <c r="B68" s="46" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="C68" s="45" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="D68" s="44" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="E68" s="45"/>
       <c r="F68" s="47"/>
@@ -5067,13 +5085,13 @@
         <v>36</v>
       </c>
       <c r="B69" s="46" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C69" s="45" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D69" s="44" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="E69" s="45"/>
       <c r="F69" s="47"/>
@@ -5093,13 +5111,13 @@
         <v>37</v>
       </c>
       <c r="B71" s="42" t="s">
-        <v>645</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>645</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>643</v>
+        <v>637</v>
+      </c>
+      <c r="C71" s="60" t="s">
+        <v>388</v>
+      </c>
+      <c r="D71" s="62" t="s">
+        <v>562</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="6"/>
@@ -5110,13 +5128,13 @@
         <v>37</v>
       </c>
       <c r="B72" s="42" t="s">
-        <v>646</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>646</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>644</v>
+        <v>638</v>
+      </c>
+      <c r="C72" s="60" t="s">
+        <v>389</v>
+      </c>
+      <c r="D72" s="62" t="s">
+        <v>563</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="6"/>
@@ -5127,13 +5145,13 @@
         <v>37</v>
       </c>
       <c r="B73" s="42" t="s">
-        <v>647</v>
-      </c>
-      <c r="C73" s="43" t="s">
-        <v>647</v>
-      </c>
-      <c r="D73" s="42" t="s">
-        <v>647</v>
+        <v>639</v>
+      </c>
+      <c r="C73" s="61" t="s">
+        <v>645</v>
+      </c>
+      <c r="D73" s="63" t="s">
+        <v>645</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="6"/>
@@ -5141,7 +5159,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>388</v>
@@ -5150,7 +5168,7 @@
         <v>388</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="6"/>
@@ -5158,7 +5176,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>389</v>
@@ -5167,7 +5185,7 @@
         <v>389</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="6"/>
@@ -5175,16 +5193,16 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B76" s="42" t="s">
-        <v>647</v>
-      </c>
-      <c r="C76" s="43" t="s">
-        <v>647</v>
-      </c>
-      <c r="D76" s="42" t="s">
-        <v>647</v>
+        <v>639</v>
+      </c>
+      <c r="C76" s="61" t="s">
+        <v>645</v>
+      </c>
+      <c r="D76" s="63" t="s">
+        <v>645</v>
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="6"/>
@@ -5201,7 +5219,7 @@
         <v>341</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="6"/>
@@ -5218,7 +5236,7 @@
         <v>342</v>
       </c>
       <c r="D78" s="55" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="6"/>
@@ -5235,7 +5253,7 @@
         <v>343</v>
       </c>
       <c r="D79" s="55" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="6"/>
@@ -5252,7 +5270,7 @@
         <v>344</v>
       </c>
       <c r="D80" s="42" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="6"/>
@@ -5269,7 +5287,7 @@
         <v>345</v>
       </c>
       <c r="D81" s="42" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="6"/>
@@ -5286,7 +5304,7 @@
         <v>346</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="6"/>
@@ -5303,7 +5321,7 @@
         <v>347</v>
       </c>
       <c r="D83" s="42" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="6"/>
@@ -5320,7 +5338,7 @@
         <v>348</v>
       </c>
       <c r="D84" s="42" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="6"/>
@@ -5331,13 +5349,13 @@
         <v>40</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="E85" s="5"/>
       <c r="F85" s="6"/>
@@ -5354,7 +5372,7 @@
         <v>333</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="E86" s="5"/>
       <c r="F86" s="6"/>
@@ -5371,7 +5389,7 @@
         <v>349</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="E87" s="5"/>
       <c r="F87" s="6"/>
@@ -5388,7 +5406,7 @@
         <v>350</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="E88" s="5"/>
       <c r="F88" s="6"/>
@@ -5405,7 +5423,7 @@
         <v>351</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E89" s="7"/>
       <c r="G89" s="6"/>
@@ -5416,31 +5434,31 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="E91" s="7"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>603</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>605</v>
+        <v>599</v>
+      </c>
+      <c r="D92" s="64" t="s">
+        <v>644</v>
       </c>
       <c r="E92" s="7"/>
     </row>
@@ -5583,7 +5601,7 @@
         <v>326</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>196</v>
@@ -5602,7 +5620,7 @@
         <v>327</v>
       </c>
       <c r="D104" s="16" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>222</v>
@@ -5621,7 +5639,7 @@
         <v>328</v>
       </c>
       <c r="D105" s="16" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>248</v>
@@ -5640,7 +5658,7 @@
         <v>85</v>
       </c>
       <c r="D106" s="16" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>57</v>
@@ -5659,7 +5677,7 @@
         <v>325</v>
       </c>
       <c r="D107" s="16" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E107" s="16" t="s">
         <v>57</v>
@@ -5678,7 +5696,7 @@
         <v>329</v>
       </c>
       <c r="D108" s="16" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>272</v>
@@ -5697,7 +5715,7 @@
         <v>330</v>
       </c>
       <c r="D109" s="16" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>298</v>
@@ -5716,7 +5734,7 @@
         <v>113</v>
       </c>
       <c r="D110" s="16" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>112</v>
@@ -5735,7 +5753,7 @@
         <v>141</v>
       </c>
       <c r="D111" s="16" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>140</v>
@@ -5754,7 +5772,7 @@
         <v>170</v>
       </c>
       <c r="D112" s="16" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>140</v>
@@ -13935,12 +13953,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>395</v>

</xml_diff>